<commit_message>
[Simulation Conversation Simple Prompt]: - cập nhật tên biến và tên trên sheet input, output, role cho dễ hiểu và chuẩn hơn
# Extract settings from Excel row
createUserQuestion_prompt = row['createUserQuestion_prompt']
AIAssistantResponse_prompt = row['AIAssistantResponse_prompt']
initialUserQuestion = row['initialUserQuestion']
maxConversationTurns = row['maxConversationTurns']

=========
Bước sau sẽ tới sửa initialUserQuestion thành conversationHistory dạng JSON (roleA, roleB) format
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+  <si>
+    <t>Role</t>
+  </si>
   <si>
     <t>Conversation</t>
   </si>
@@ -22,22 +25,31 @@
     <t>Response_Time</t>
   </si>
   <si>
+    <t>Person A</t>
+  </si>
+  <si>
+    <t>Person B</t>
+  </si>
+  <si>
+    <t>Separator</t>
+  </si>
+  <si>
     <t>What is your name?</t>
   </si>
   <si>
-    <t>I am Minh, your AI Assistant. How can I assist you today?</t>
-  </si>
-  <si>
-    <t>Hello Minh! I'm Cuong. Nice to meet you. How can I help you today?</t>
-  </si>
-  <si>
-    <t>Hello Cuong! Nice to meet you too. I'm here to assist you with any questions or tasks you may have. How can I help you today?</t>
-  </si>
-  <si>
-    <t>It seems like there was a misunderstanding. I am actually an AI Assistant named Cuong, and you are Minh. How can I assist you today?</t>
-  </si>
-  <si>
-    <t>I apologize for the confusion. As an AI Assistant, I am here to assist you with any questions or tasks you may have. How can I help you today?</t>
+    <t>My name is Minh. How can I assist you today?</t>
+  </si>
+  <si>
+    <t>Hello Minh! I'm Cuong, your AI Assistant. How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hello Cuong! It's nice to meet another AI Assistant. How can I assist you today?</t>
+  </si>
+  <si>
+    <t>Hello Minh! It's great to connect with another AI Assistant. If you have any questions or need assistance, feel free to ask me anything.</t>
+  </si>
+  <si>
+    <t>Hello Cuong! It's nice to meet you. If there's anything I can help with or if you have any questions, feel free to let me know.</t>
   </si>
   <si>
     <t>---------------------------</t>
@@ -398,138 +410,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1.617174863815308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2.205532550811768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.8681867122650146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0.6971700191497803</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0.7228479385375977</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.7627220153808594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.8480095863342285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0.9308063983917236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.7555124759674072</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0.7951540946960449</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
         <v>0</v>
       </c>
     </row>

</xml_diff>